<commit_message>
Seguimiento CS_10_CO a 18/03/2015 12:57 m
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -68,10 +68,10 @@
     <t>En revisión de María Clemencia</t>
   </si>
   <si>
-    <t>En corrección Mabel</t>
-  </si>
-  <si>
     <t>Estoy revisando los mapas elaborados por la documentadora</t>
+  </si>
+  <si>
+    <t>Ya puede ser revisado por María Clemencia</t>
   </si>
 </sst>
 </file>
@@ -530,6 +530,9 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -556,9 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,7 +843,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.25"/>
@@ -864,15 +864,15 @@
       <c r="B1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
       <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickBot="1">
       <c r="B3" s="26"/>
@@ -880,31 +880,31 @@
       <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="31" t="s">
+      <c r="J4" s="40"/>
+      <c r="K4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="31"/>
+      <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="45.75" thickBot="1">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
@@ -958,11 +958,11 @@
       <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="31">
         <v>42072</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
@@ -974,14 +974,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="5">
-        <v>42076</v>
-      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="18"/>
@@ -1069,15 +1065,25 @@
       <c r="K12" s="14"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:12" ht="16.5" thickBot="1">
+    <row r="13" spans="1:12" ht="29.25" thickBot="1">
       <c r="A13" s="29">
         <v>8</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
+      <c r="B13" s="4">
+        <v>42075</v>
+      </c>
+      <c r="C13" s="5">
+        <v>42081</v>
+      </c>
+      <c r="D13" s="5">
+        <v>42081</v>
+      </c>
+      <c r="E13" s="5">
+        <v>42053</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
       <c r="I13" s="18"/>

</xml_diff>

<commit_message>
Seguimiento actualizado a 19-03-2015
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -843,7 +843,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.25"/>
@@ -973,7 +973,9 @@
       <c r="A7" s="29">
         <v>2</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4">
+        <v>42082</v>
+      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>

</xml_diff>

<commit_message>
Seguimiento actualizado a 25-03-2015
Seguimiento actualizado con la unidad 2
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Editorial</t>
   </si>
@@ -843,7 +843,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.25"/>
@@ -969,17 +969,25 @@
       <c r="K6" s="14"/>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" thickBot="1">
+    <row r="7" spans="1:12" ht="29.25" thickBot="1">
       <c r="A7" s="29">
         <v>2</v>
       </c>
       <c r="B7" s="4">
         <v>42082</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="5">
+        <v>42088</v>
+      </c>
+      <c r="D7" s="5">
+        <v>42088</v>
+      </c>
+      <c r="E7" s="5">
+        <v>42088</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="18"/>

</xml_diff>

<commit_message>
Archivo de seguimiento grado 10 a 27/04/2015
Seguimiento actualizado
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Editorial</t>
   </si>
@@ -68,10 +68,16 @@
     <t>En revisión de María Clemencia</t>
   </si>
   <si>
-    <t>Estoy revisando los mapas elaborados por la documentadora</t>
-  </si>
-  <si>
-    <t>Ya puede ser revisado por María Clemencia</t>
+    <t>Se van a incluir nuevas imágenes</t>
+  </si>
+  <si>
+    <t>Está siendo reestructurada</t>
+  </si>
+  <si>
+    <t>Entregada por la autora para edición</t>
+  </si>
+  <si>
+    <t>Entregada por el autor para edición</t>
   </si>
 </sst>
 </file>
@@ -843,7 +849,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.25"/>
@@ -939,7 +945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.5" thickBot="1">
+    <row r="6" spans="1:12" ht="29.25" thickBot="1">
       <c r="A6" s="29">
         <v>1</v>
       </c>
@@ -988,22 +994,32 @@
       <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="31">
+        <v>42078</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="I7" s="18"/>
       <c r="J7" s="19"/>
       <c r="K7" s="14"/>
       <c r="L7" s="15"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5" thickBot="1">
+    <row r="8" spans="1:12" ht="29.25" thickBot="1">
       <c r="A8" s="29">
         <v>3</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="4">
+        <v>42118</v>
+      </c>
+      <c r="C8" s="5">
+        <v>42118</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
       <c r="I8" s="18"/>
@@ -1101,15 +1117,21 @@
       <c r="K13" s="14"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" thickBot="1">
+    <row r="14" spans="1:12" ht="29.25" thickBot="1">
       <c r="A14" s="29">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="4">
+        <v>42121</v>
+      </c>
+      <c r="C14" s="5">
+        <v>42121</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G14" s="10"/>
       <c r="H14" s="11"/>
       <c r="I14" s="18"/>

</xml_diff>

<commit_message>
Seguimiento actualizado a 04/05/2015
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Editorial</t>
   </si>
@@ -68,16 +68,16 @@
     <t>En revisión de María Clemencia</t>
   </si>
   <si>
-    <t>Se van a incluir nuevas imágenes</t>
-  </si>
-  <si>
     <t>Está siendo reestructurada</t>
   </si>
   <si>
-    <t>Entregada por la autora para edición</t>
-  </si>
-  <si>
     <t>Entregada por el autor para edición</t>
+  </si>
+  <si>
+    <t>Manuscrito listo para revisión de María Clemencia</t>
+  </si>
+  <si>
+    <t>Imágenes corregidas por documentadora</t>
   </si>
 </sst>
 </file>
@@ -849,7 +849,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="14.25"/>
@@ -965,10 +965,10 @@
         <v>13</v>
       </c>
       <c r="G6" s="31">
-        <v>42072</v>
+        <v>42124</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
@@ -992,13 +992,13 @@
         <v>42088</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="31">
-        <v>42078</v>
+        <v>42128</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="19"/>
@@ -1018,7 +1018,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
@@ -1108,16 +1108,20 @@
         <v>42053</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="G13" s="31">
+        <v>42122</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="I13" s="18"/>
       <c r="J13" s="19"/>
       <c r="K13" s="14"/>
       <c r="L13" s="15"/>
     </row>
-    <row r="14" spans="1:12" ht="29.25" thickBot="1">
+    <row r="14" spans="1:12" ht="43.5" thickBot="1">
       <c r="A14" s="29">
         <v>9</v>
       </c>

</xml_diff>